<commit_message>
multiprocessing for data collection
</commit_message>
<xml_diff>
--- a/chords.xlsx
+++ b/chords.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user1/Desktop/CS/cs428/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{B172EDB8-ADD4-294C-A137-40AE314312E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01E9CB49-7792-FD43-8DB6-E12858F795ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16580"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="chords" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="110">
   <si>
     <t>A</t>
   </si>
@@ -268,21 +268,12 @@
     <t>032030</t>
   </si>
   <si>
-    <t>Amaj7</t>
-  </si>
-  <si>
     <t>002120</t>
   </si>
   <si>
-    <t>Dmaj7</t>
-  </si>
-  <si>
     <t>000222</t>
   </si>
   <si>
-    <t>Gmaj7</t>
-  </si>
-  <si>
     <t>320002</t>
   </si>
   <si>
@@ -292,15 +283,9 @@
     <t>320000</t>
   </si>
   <si>
-    <t>Emaj7</t>
-  </si>
-  <si>
     <t>021100</t>
   </si>
   <si>
-    <t>Cmaj7</t>
-  </si>
-  <si>
     <t>032000</t>
   </si>
   <si>
@@ -328,22 +313,49 @@
     <t>000211</t>
   </si>
   <si>
-    <t>Ammaj7</t>
-  </si>
-  <si>
     <t>002110</t>
   </si>
   <si>
-    <t>Emmaj7</t>
-  </si>
-  <si>
     <t>021000</t>
+  </si>
+  <si>
+    <t>Am(maj7)</t>
+  </si>
+  <si>
+    <t>Em(maj7)</t>
+  </si>
+  <si>
+    <t>A(maj7)</t>
+  </si>
+  <si>
+    <t>D(maj7)</t>
+  </si>
+  <si>
+    <t>G(maj7)</t>
+  </si>
+  <si>
+    <t>E(maj7)</t>
+  </si>
+  <si>
+    <t>C(maj7)</t>
+  </si>
+  <si>
+    <t>B7</t>
+  </si>
+  <si>
+    <t>021202</t>
+  </si>
+  <si>
+    <t>Bm7</t>
+  </si>
+  <si>
+    <t>020202</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1197,11 +1209,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B64"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F61" sqref="F61"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1559,103 +1571,119 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
+        <v>101</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>84</v>
+        <v>102</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>86</v>
+        <v>103</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>90</v>
+        <v>104</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>95</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>96</v>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>106</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>97</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>99</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>100</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>108</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>